<commit_message>
Refactored: Change path log4j.properties resource to resources
</commit_message>
<xml_diff>
--- a/src/main/resource/facebook.xlsx
+++ b/src/main/resource/facebook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Altamash\IdeaProjects\OpenPageModelFramwork\src\main\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B6A692-9CE8-4CBD-A445-02FECDBB8EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D987ABD5-239B-4741-A130-8E4C0B8744D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{85D43113-1378-48E3-8F9D-9691B85BD259}"/>
   </bookViews>
@@ -50,7 +50,7 @@
     <t>8109555221</t>
   </si>
   <si>
-    <t>Qais@7744</t>
+    <t>Qais@774493</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Added: Functioning of perform take screenshot when test failed by using WebEventListener
</commit_message>
<xml_diff>
--- a/src/main/resource/facebook.xlsx
+++ b/src/main/resource/facebook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Altamash\IdeaProjects\OpenPageModelFramwork\src\main\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D987ABD5-239B-4741-A130-8E4C0B8744D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F0ABAC-8266-4565-865C-91C9E880A611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{85D43113-1378-48E3-8F9D-9691B85BD259}"/>
   </bookViews>
@@ -50,7 +50,7 @@
     <t>8109555221</t>
   </si>
   <si>
-    <t>Qais@774493</t>
+    <t>Qais@313</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Added: More pages inside Profile Pages in POM framework Facebook
</commit_message>
<xml_diff>
--- a/src/main/resource/facebook.xlsx
+++ b/src/main/resource/facebook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Altamash\IdeaProjects\OpenPageModelFramwork\src\main\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F0ABAC-8266-4565-865C-91C9E880A611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B6DAE35-4EE9-4DBA-9633-C63229B994EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{85D43113-1378-48E3-8F9D-9691B85BD259}"/>
   </bookViews>
@@ -50,7 +50,7 @@
     <t>8109555221</t>
   </si>
   <si>
-    <t>Qais@313</t>
+    <t>Qais@720</t>
   </si>
 </sst>
 </file>

</xml_diff>